<commit_message>
Artcile add the Super model table and notes
</commit_message>
<xml_diff>
--- a/results-latex-tables/LaTex_Table_Formatter_V4.4_08-Jul-2023.xlsx
+++ b/results-latex-tables/LaTex_Table_Formatter_V4.4_08-Jul-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\HEI\P-4 Research Phase\Empirical_Study_REINFORCE\results-latex-tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\results-latex-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F68DC9-56FF-4BD3-8901-59F50177EF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D224C551-26F5-44F7-9D71-0E90C07F7E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="436" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="436" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LATEX" sheetId="27" r:id="rId1"/>
@@ -22,24 +22,11 @@
     <sheet name="t-test" sheetId="35" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="140">
   <si>
     <t>environment_info</t>
   </si>
@@ -383,9 +370,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>Abstract</t>
-  </si>
-  <si>
     <t>Pr</t>
   </si>
   <si>
@@ -474,6 +458,18 @@
   </si>
   <si>
     <t>Metric</t>
+  </si>
+  <si>
+    <t>Rc</t>
+  </si>
+  <si>
+    <t>F0.5</t>
+  </si>
+  <si>
+    <t>Supermodels</t>
+  </si>
+  <si>
+    <t>Abstract and super-model sections</t>
   </si>
 </sst>
 </file>
@@ -717,7 +713,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,8 +935,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1075,6 +1077,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1120,7 +1131,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1174,6 +1185,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="26" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1875,7 +1890,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
@@ -5041,10 +5056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905A37E9-AAF7-4185-BB7B-87043DE103AD}">
-  <dimension ref="B1:O40"/>
+  <dimension ref="B1:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6061,6 +6076,11 @@
       <c r="O40" s="16" t="str">
         <f>_xlfn.CONCAT(TEXT(B40, "0.000"), " &amp; ",  TEXT(C40, "0.000"), " &amp; ",TEXT( D40,  "0.000"), " &amp; &amp;", TEXT(F40,  "0.000"), " &amp; ",TEXT(G40, "0.000"), " &amp; &amp; ", TEXT(I40,  "0.000"), " &amp; ", TEXT(J40, "0.000"), " &amp; &amp;",  TEXT(L40,  "0.000"), " &amp;", TEXT(M40,  "0.000"), " \\")</f>
         <v>REINFORCE &amp; 0.813 &amp; 0.119 &amp; &amp;0.421 &amp; 0.079 &amp; &amp; 0.495 &amp; 0.090 &amp; &amp;0.609 &amp;0.101 \\</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -6476,7 +6496,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="27" x14ac:dyDescent="0.35">
       <c r="B1" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
@@ -9090,17 +9110,28 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBC427A-C68D-45FE-989E-74DC87A3B6CF}">
-  <dimension ref="A2:AH25"/>
+  <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2:AH17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" customWidth="1"/>
+    <col min="15" max="18" width="9.140625" customWidth="1"/>
+    <col min="23" max="26" width="9.140625" customWidth="1"/>
+    <col min="31" max="35" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="AD1" s="36"/>
+    </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
@@ -9117,7 +9148,7 @@
       <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="37" t="s">
         <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -9141,7 +9172,7 @@
       <c r="M2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="37" t="s">
         <v>53</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -9165,7 +9196,7 @@
       <c r="U2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="37" t="s">
         <v>55</v>
       </c>
       <c r="W2" s="1" t="s">
@@ -9189,7 +9220,7 @@
       <c r="AC2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="37" t="s">
         <v>57</v>
       </c>
       <c r="AE2" s="1" t="s">
@@ -9221,7 +9252,7 @@
       <c r="E3" s="1">
         <v>0.92604813601977498</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="37">
         <v>0.90786648456907004</v>
       </c>
       <c r="G3" s="1">
@@ -9245,7 +9276,7 @@
       <c r="M3" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="37">
         <v>0.55555555555555503</v>
       </c>
       <c r="O3" s="1">
@@ -9269,7 +9300,7 @@
       <c r="U3" s="1">
         <v>0.66680512649244295</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="37">
         <v>0.55962256570240099</v>
       </c>
       <c r="W3" s="1">
@@ -9293,7 +9324,7 @@
       <c r="AC3" s="1">
         <v>0.51847883597883604</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AD3" s="37">
         <v>0.59674369747899103</v>
       </c>
       <c r="AE3" s="1">
@@ -9325,7 +9356,7 @@
       <c r="E4" s="1">
         <v>0.95202889964122295</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="37">
         <v>0.95689659977703401</v>
       </c>
       <c r="G4" s="1">
@@ -9349,7 +9380,7 @@
       <c r="M4" s="1">
         <v>0.68042285726004004</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="37">
         <v>0.57100489949327105</v>
       </c>
       <c r="O4" s="1">
@@ -9373,7 +9404,7 @@
       <c r="U4" s="1">
         <v>0.66212741087083504</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="37">
         <v>0.55428558844256504</v>
       </c>
       <c r="W4" s="1">
@@ -9397,7 +9428,7 @@
       <c r="AC4" s="1">
         <v>0.53017502893152002</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AD4" s="37">
         <v>0.58643350625216395</v>
       </c>
       <c r="AE4" s="1">
@@ -9429,7 +9460,7 @@
       <c r="E5" s="1">
         <v>0.95456567539097303</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="37">
         <v>0.93489621489621499</v>
       </c>
       <c r="G5" s="1">
@@ -9453,7 +9484,7 @@
       <c r="M5" s="1">
         <v>0.66892655367231602</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="37">
         <v>0.55808080808080796</v>
       </c>
       <c r="O5" s="1">
@@ -9477,7 +9508,7 @@
       <c r="U5" s="1">
         <v>0.66781609195402303</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="37">
         <v>0.55876350716466905</v>
       </c>
       <c r="W5" s="1">
@@ -9501,7 +9532,7 @@
       <c r="AC5" s="1">
         <v>0.433790051911494</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AD5" s="37">
         <v>0.50451726743328895</v>
       </c>
       <c r="AE5" s="1">
@@ -9533,7 +9564,7 @@
       <c r="E6" s="1">
         <v>0.93885962779893495</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="37">
         <v>0.90839947089947004</v>
       </c>
       <c r="G6" s="1">
@@ -9557,7 +9588,7 @@
       <c r="M6" s="1">
         <v>0.602917629842876</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="37">
         <v>0.59232381748686103</v>
       </c>
       <c r="O6" s="1">
@@ -9581,7 +9612,7 @@
       <c r="U6" s="1">
         <v>0.77587454981992798</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="37">
         <v>0.69294096426449303</v>
       </c>
       <c r="W6" s="1">
@@ -9605,7 +9636,7 @@
       <c r="AC6" s="1">
         <v>0.70343570525058696</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AD6" s="37">
         <v>0.59735727340662104</v>
       </c>
       <c r="AE6" s="1">
@@ -9637,7 +9668,7 @@
       <c r="E7" s="1">
         <v>0.86076036432073499</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="37">
         <v>0.93237715913631203</v>
       </c>
       <c r="G7" s="1">
@@ -9661,7 +9692,7 @@
       <c r="M7" s="1">
         <v>0.66440677966101602</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="37">
         <v>0.55397727272727204</v>
       </c>
       <c r="O7" s="1">
@@ -9685,7 +9716,7 @@
       <c r="U7" s="1">
         <v>0.66779661016949099</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="37">
         <v>0.55871212121212099</v>
       </c>
       <c r="W7" s="1">
@@ -9709,7 +9740,7 @@
       <c r="AC7" s="1">
         <v>0.675443924070534</v>
       </c>
-      <c r="AD7" s="1">
+      <c r="AD7" s="37">
         <v>0.64287979046043497</v>
       </c>
       <c r="AE7" s="1">
@@ -9741,7 +9772,7 @@
       <c r="E8" s="1">
         <v>0.90530341908674195</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="37">
         <v>0.87137602978120199</v>
       </c>
       <c r="G8" s="1">
@@ -9765,7 +9796,7 @@
       <c r="M8" s="1">
         <v>0.58802954183720302</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="37">
         <v>0.54562208866051298</v>
       </c>
       <c r="O8" s="1">
@@ -9789,7 +9820,7 @@
       <c r="U8" s="1">
         <v>0.66789401909214796</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="37">
         <v>0.55982793046746504</v>
       </c>
       <c r="W8" s="1">
@@ -9813,7 +9844,7 @@
       <c r="AC8" s="1">
         <v>0.60435461548904901</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AD8" s="37">
         <v>0.55070744403944405</v>
       </c>
       <c r="AE8" s="1">
@@ -9845,7 +9876,7 @@
       <c r="E9" s="1">
         <v>0.89512516469038195</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="37">
         <v>0.84232480533926601</v>
       </c>
       <c r="G9" s="1">
@@ -9869,7 +9900,7 @@
       <c r="M9" s="1">
         <v>0.58327472086143195</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="37">
         <v>0.55364531302031295</v>
       </c>
       <c r="O9" s="1">
@@ -9893,7 +9924,7 @@
       <c r="U9" s="1">
         <v>0.65964912280701704</v>
       </c>
-      <c r="V9" s="1">
+      <c r="V9" s="37">
         <v>0.55447225578039505</v>
       </c>
       <c r="W9" s="1">
@@ -9917,7 +9948,7 @@
       <c r="AC9" s="1">
         <v>0.70237621100449599</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AD9" s="37">
         <v>0.62244089900339905</v>
       </c>
       <c r="AE9" s="1">
@@ -9949,7 +9980,7 @@
       <c r="E10" s="1">
         <v>0.87929191882249902</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="37">
         <v>0.82880366412415896</v>
       </c>
       <c r="G10" s="1">
@@ -9973,7 +10004,7 @@
       <c r="M10" s="1">
         <v>0.60260514117513597</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="37">
         <v>0.57326781076327604</v>
       </c>
       <c r="O10" s="1">
@@ -9997,7 +10028,7 @@
       <c r="U10" s="1">
         <v>0.84259944495837102</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="37">
         <v>0.77364369501466201</v>
       </c>
       <c r="W10" s="1">
@@ -10021,7 +10052,7 @@
       <c r="AC10" s="1">
         <v>0.59583761620042397</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AD10" s="37">
         <v>0.56471270069330404</v>
       </c>
       <c r="AE10" s="1">
@@ -10053,7 +10084,7 @@
       <c r="E11" s="1">
         <v>0.76652274250858599</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="37">
         <v>0.73006565837141402</v>
       </c>
       <c r="G11" s="1">
@@ -10077,7 +10108,7 @@
       <c r="M11" s="1">
         <v>0.640826339570996</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="37">
         <v>0.56297323702751301</v>
       </c>
       <c r="O11" s="1">
@@ -10101,7 +10132,7 @@
       <c r="U11" s="1">
         <v>0.67245480738667196</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="37">
         <v>0.56498645088761301</v>
       </c>
       <c r="W11" s="1">
@@ -10125,7 +10156,7 @@
       <c r="AC11" s="1">
         <v>0.63321424788366498</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AD11" s="37">
         <v>0.55811900482138999</v>
       </c>
       <c r="AE11" s="1">
@@ -10157,7 +10188,7 @@
       <c r="E12" s="1">
         <v>0.94395083342451702</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="37">
         <v>0.97662631752305595</v>
       </c>
       <c r="G12" s="1">
@@ -10181,7 +10212,7 @@
       <c r="M12" s="1">
         <v>0.58732131542225796</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="37">
         <v>0.54486445710434295</v>
       </c>
       <c r="O12" s="1">
@@ -10205,7 +10236,7 @@
       <c r="U12" s="1">
         <v>0.95397023471895803</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V12" s="37">
         <v>0.942314306064306</v>
       </c>
       <c r="W12" s="1">
@@ -10229,7 +10260,7 @@
       <c r="AC12" s="1">
         <v>0.61487124797331605</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AD12" s="37">
         <v>0.59725202264557498</v>
       </c>
       <c r="AE12" s="1">
@@ -10261,7 +10292,7 @@
       <c r="E13" s="1">
         <v>0.86111015584699702</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="37">
         <v>0.90779985413137598</v>
       </c>
       <c r="G13" s="1">
@@ -10285,7 +10316,7 @@
       <c r="M13" s="1">
         <v>0.66779661016949099</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="37">
         <v>0.55681818181818099</v>
       </c>
       <c r="O13" s="1">
@@ -10309,7 +10340,7 @@
       <c r="U13" s="1">
         <v>0.82552839317545101</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="37">
         <v>0.90147243107769404</v>
       </c>
       <c r="W13" s="1">
@@ -10333,7 +10364,7 @@
       <c r="AC13" s="1">
         <v>0.437812018995962</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AD13" s="37">
         <v>0.49735387619439902</v>
       </c>
       <c r="AE13" s="1">
@@ -10356,16 +10387,16 @@
       <c r="B14" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="35">
         <v>0.82074371534897805</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="35">
         <v>0.84499999999999997</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="35">
         <v>0.83145452963809796</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="37">
         <v>0.82471427747664605</v>
       </c>
       <c r="G14" s="1">
@@ -10389,7 +10420,7 @@
       <c r="M14" s="1">
         <v>0.62823946392830599</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="37">
         <v>0.57200429178642198</v>
       </c>
       <c r="O14" s="1">
@@ -10404,16 +10435,16 @@
       <c r="R14" s="1">
         <v>6.98933772204888E-2</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="35">
         <v>0.98015873015873001</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="35">
         <v>0.96</v>
       </c>
-      <c r="U14" s="1">
+      <c r="U14" s="35">
         <v>0.96933609821928102</v>
       </c>
-      <c r="V14" s="1">
+      <c r="V14" s="37">
         <v>0.97564450947603099</v>
       </c>
       <c r="W14" s="1">
@@ -10437,7 +10468,7 @@
       <c r="AC14" s="1">
         <v>0.56353269465529698</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AD14" s="37">
         <v>0.537350620324758</v>
       </c>
       <c r="AE14" s="1">
@@ -10469,7 +10500,7 @@
       <c r="E15" s="1">
         <v>0.90289497604967694</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="37">
         <v>0.85568621219344199</v>
       </c>
       <c r="G15" s="1">
@@ -10493,7 +10524,7 @@
       <c r="M15" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="37">
         <v>0.55555555555555503</v>
       </c>
       <c r="O15" s="1">
@@ -10517,7 +10548,7 @@
       <c r="U15" s="1">
         <v>0.66787658802177796</v>
       </c>
-      <c r="V15" s="1">
+      <c r="V15" s="37">
         <v>0.55982478438873695</v>
       </c>
       <c r="W15" s="1">
@@ -10541,7 +10572,7 @@
       <c r="AC15" s="1">
         <v>0.54885442832833597</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="AD15" s="37">
         <v>0.52562617937617895</v>
       </c>
       <c r="AE15" s="1">
@@ -10573,7 +10604,7 @@
       <c r="E16" s="1">
         <v>0.576977653006574</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="37">
         <v>0.73760874542124499</v>
       </c>
       <c r="G16" s="1">
@@ -10597,7 +10628,7 @@
       <c r="M16" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="37">
         <v>0.55555555555555503</v>
       </c>
       <c r="O16" s="1">
@@ -10621,7 +10652,7 @@
       <c r="U16" s="1">
         <v>0.662049483732709</v>
       </c>
-      <c r="V16" s="1">
+      <c r="V16" s="37">
         <v>0.55520424343098695</v>
       </c>
       <c r="W16" s="1">
@@ -10645,7 +10676,7 @@
       <c r="AC16" s="1">
         <v>0.55797894096120904</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="AD16" s="37">
         <v>0.521793376763942</v>
       </c>
       <c r="AE16" s="1">
@@ -10677,7 +10708,7 @@
       <c r="E17" s="1">
         <v>0.89618266717111295</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="37">
         <v>0.91791018964932003</v>
       </c>
       <c r="G17" s="1">
@@ -10701,7 +10732,7 @@
       <c r="M17" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="37">
         <v>0.55555555555555503</v>
       </c>
       <c r="O17" s="1">
@@ -10725,7 +10756,7 @@
       <c r="U17" s="1">
         <v>0.74090909090909096</v>
       </c>
-      <c r="V17" s="1">
+      <c r="V17" s="37">
         <v>0.86274509803921495</v>
       </c>
       <c r="W17" s="1">
@@ -10749,7 +10780,7 @@
       <c r="AC17" s="1">
         <v>0.57673058143902101</v>
       </c>
-      <c r="AD17" s="1">
+      <c r="AD17" s="37">
         <v>0.52618412783874402</v>
       </c>
       <c r="AE17" s="1">
@@ -10769,7 +10800,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -10777,7 +10808,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -10785,7 +10816,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
+      <c r="V18" s="37"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -10793,7 +10824,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
+      <c r="AD18" s="37"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
@@ -10812,7 +10843,7 @@
         <f t="shared" si="0"/>
         <v>0.87273845089445501</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="37">
         <f t="shared" si="0"/>
         <v>0.87555677888594841</v>
       </c>
@@ -10844,7 +10875,7 @@
         <f t="shared" si="0"/>
         <v>0.63876224133784898</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="37">
         <f t="shared" si="0"/>
         <v>0.56045362667939957</v>
       </c>
@@ -10876,7 +10907,7 @@
         <f t="shared" si="0"/>
         <v>0.74017913815521308</v>
       </c>
-      <c r="V19" s="1">
+      <c r="V19" s="37">
         <f t="shared" si="0"/>
         <v>0.67829736342755687</v>
       </c>
@@ -10908,7 +10939,7 @@
         <f t="shared" si="0"/>
         <v>0.57979240993824988</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AD19" s="37">
         <f t="shared" si="0"/>
         <v>0.56196478578217568</v>
       </c>
@@ -10933,7 +10964,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -10941,7 +10972,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -10949,7 +10980,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
+      <c r="V20" s="37"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -10957,24 +10988,20 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
+      <c r="AD20" s="37"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>108</v>
-      </c>
+      <c r="B21" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -10982,7 +11009,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="N21" s="37"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -10990,7 +11017,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
+      <c r="V21" s="37"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -10998,34 +11025,32 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
+      <c r="AD21" s="37"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="1">
-        <f>C19</f>
-        <v>0.88392420394707583</v>
-      </c>
-      <c r="D22" s="1">
-        <f>E19</f>
-        <v>0.87273845089445501</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="C22" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>137</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="N22" s="37"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -11033,7 +11058,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
+      <c r="V22" s="37"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -11041,34 +11066,20 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
+      <c r="AD22" s="37"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1">
-        <f>K19</f>
-        <v>0.51997246637140981</v>
-      </c>
-      <c r="D23" s="1">
-        <f>M19</f>
-        <v>0.63876224133784898</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="N23" s="37"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -11076,7 +11087,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
+      <c r="V23" s="37"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -11084,7 +11095,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
+      <c r="AD23" s="37"/>
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
@@ -11092,26 +11103,31 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
-        <f>S19</f>
-        <v>0.65086105665750416</v>
-      </c>
-      <c r="D24" s="1">
-        <f>U19</f>
-        <v>0.74017913815521308</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+        <f>K19</f>
+        <v>0.51997246637140981</v>
+      </c>
+      <c r="E24" s="1">
+        <f>L19</f>
+        <v>0.85866666666666658</v>
+      </c>
+      <c r="F24" s="1">
+        <f>M19</f>
+        <v>0.63876224133784898</v>
+      </c>
+      <c r="G24" s="37">
+        <f>N19</f>
+        <v>0.56045362667939957</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+      <c r="N24" s="37"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -11119,7 +11135,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
+      <c r="V24" s="37"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -11127,7 +11143,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
+      <c r="AD24" s="37"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
@@ -11135,26 +11151,31 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
-        <f>AA19</f>
-        <v>0.55800190542581041</v>
-      </c>
-      <c r="D25" s="1">
-        <f>AC19</f>
-        <v>0.57979240993824988</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+        <f>S19</f>
+        <v>0.65086105665750416</v>
+      </c>
+      <c r="E25" s="1">
+        <f>T19</f>
+        <v>0.93699999999999994</v>
+      </c>
+      <c r="F25" s="1">
+        <f>U19</f>
+        <v>0.74017913815521308</v>
+      </c>
+      <c r="G25" s="37">
+        <f>V19</f>
+        <v>0.67829736342755687</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -11162,7 +11183,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
+      <c r="V25" s="37"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -11170,14 +11191,129 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
+      <c r="AD25" s="37"/>
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1">
+        <f>AA19</f>
+        <v>0.55800190542581041</v>
+      </c>
+      <c r="E26" s="1">
+        <f>AB19</f>
+        <v>0.64266666666666661</v>
+      </c>
+      <c r="F26" s="1">
+        <f>AC19</f>
+        <v>0.57979240993824988</v>
+      </c>
+      <c r="G26" s="37">
+        <f>AD19</f>
+        <v>0.56196478578217568</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="37"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1">
+        <f>C19</f>
+        <v>0.88392420394707583</v>
+      </c>
+      <c r="E27" s="1">
+        <f>D19</f>
+        <v>0.8843333333333333</v>
+      </c>
+      <c r="F27" s="1">
+        <f>E19</f>
+        <v>0.87273845089445501</v>
+      </c>
+      <c r="G27" s="37">
+        <f>F19</f>
+        <v>0.87555677888594841</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <f>C27-MAX(C24:C26)</f>
+        <v>0.23306314728957167</v>
+      </c>
+      <c r="E28" s="1">
+        <f>E27-MAX(E24:E26)</f>
+        <v>-5.2666666666666639E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f>F27-MAX(F24:F26)</f>
+        <v>0.13255931273924193</v>
+      </c>
+      <c r="G28" s="1">
+        <f>G27-MAX(G24:G26)</f>
+        <v>0.19725941545839154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11185,7 +11321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA18A990-26F2-4A3D-B461-CA3EE7632A75}">
   <dimension ref="B2:Q56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
@@ -11231,54 +11367,54 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="21" t="s">
         <v>113</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>119</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G8" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G9" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -11286,20 +11422,20 @@
     </row>
     <row r="11" spans="2:17" s="24" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="23"/>
       <c r="H11" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:17" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25"/>
       <c r="C12" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D12" s="26" t="s">
         <v>25</v>
@@ -11336,7 +11472,7 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13">
         <v>1500</v>
@@ -11345,13 +11481,13 @@
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="H13" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="M13" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N13" s="28"/>
       <c r="O13" s="28"/>
@@ -11446,7 +11582,7 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="28">
@@ -11459,7 +11595,7 @@
         <v>5.2915684155002098E-155</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I16" s="1">
         <v>17.3636428588526</v>
@@ -11472,7 +11608,7 @@
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N16" s="1">
         <v>0.44166807409040798</v>
@@ -11617,7 +11753,7 @@
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="28">
@@ -11630,7 +11766,7 @@
         <v>2.96294283830361E-242</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I21" s="1">
         <v>32.402190474587201</v>
@@ -11643,7 +11779,7 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N21" s="1">
         <v>0.36261981429192502</v>
@@ -11677,7 +11813,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23">
         <v>900</v>
@@ -11686,14 +11822,14 @@
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
       <c r="H23" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -11788,7 +11924,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="28">
@@ -11801,7 +11937,7 @@
         <v>2.19443258873019E-67</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I26" s="1">
         <v>9.1210560061112904</v>
@@ -11814,7 +11950,7 @@
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N26" s="1">
         <v>0.45244467580584302</v>
@@ -11848,7 +11984,7 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28">
         <v>300</v>
@@ -11857,14 +11993,14 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="H28" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -11959,7 +12095,7 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="28">
@@ -11972,7 +12108,7 @@
         <v>1.3511740966455699E-3</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="1">
         <v>0.34942564568737999</v>
@@ -11985,7 +12121,7 @@
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N31" s="1">
         <v>0.48838652874258598</v>
@@ -12002,19 +12138,19 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
       <c r="G36" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
@@ -12024,7 +12160,7 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>25</v>
@@ -12037,7 +12173,7 @@
       </c>
       <c r="F37" s="27"/>
       <c r="G37" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H37" s="26" t="s">
         <v>25</v>
@@ -12057,13 +12193,13 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
       <c r="G38" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
@@ -12140,7 +12276,7 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="28">
         <v>1.9919308224305299E-64</v>
@@ -12152,7 +12288,7 @@
         <v>5.2915684155002098E-155</v>
       </c>
       <c r="G41" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H41" s="1">
         <v>17.3636428588526</v>
@@ -12188,13 +12324,13 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="G43" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -12272,7 +12408,7 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="28">
         <v>9.5954024624663701E-134</v>
@@ -12284,7 +12420,7 @@
         <v>2.96294283830361E-242</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H46" s="1">
         <v>32.402190474587201</v>
@@ -12320,13 +12456,13 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
       <c r="E48" s="28"/>
       <c r="G48" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -12404,7 +12540,7 @@
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C51" s="28">
         <v>1.9355122289398401E-19</v>
@@ -12416,7 +12552,7 @@
         <v>2.19443258873019E-67</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H51" s="1">
         <v>9.1210560061112904</v>
@@ -12452,13 +12588,13 @@
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="28"/>
       <c r="E53" s="28"/>
       <c r="G53" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -12536,7 +12672,7 @@
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="28">
         <v>0.72689279578392996</v>
@@ -12548,7 +12684,7 @@
         <v>1.3511740966455699E-3</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H56" s="1">
         <v>0.34942564568737999</v>

</xml_diff>